<commit_message>
Version 12 noviembre 2
</commit_message>
<xml_diff>
--- a/DATOS_FINALES/Recomendaciones.xlsx
+++ b/DATOS_FINALES/Recomendaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.2\cenyt-proyectos\CEN-223_TD GUAFITA\2.INFOENTRADA\DATOS_FINALES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747E11DC-7C78-48E3-A878-944C7BB829D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67413DAF-32D9-4442-89D4-D9950E474EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="51">
   <si>
     <t>REEMPLAZO DE POSTES</t>
   </si>
@@ -45,9 +45,6 @@
     <t>NORMALIZACION ESTRUCTURA SUSPENSION 13 kv a 35 kv</t>
   </si>
   <si>
-    <t>RETIRADA / INSTALACION JUEGO DPSs DE LINEA</t>
-  </si>
-  <si>
     <t>CONSTRUCCION PUESTAS A TIERRA PARA DPSs DE LINEA</t>
   </si>
   <si>
@@ -172,13 +169,25 @@
   </si>
   <si>
     <t>Largo</t>
+  </si>
+  <si>
+    <t>MONTAR PROTECCIONES ANTINIDO</t>
+  </si>
+  <si>
+    <t>MANTENIMIENTO DE POSTES</t>
+  </si>
+  <si>
+    <t>NORMALIZACIÓN ESTRUCTURA TERMINAL 13 kV a 35 kV2</t>
+  </si>
+  <si>
+    <t>RETIRADA  JUEGO DPSs DE LINEA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +213,23 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,8 +248,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -246,11 +276,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -262,6 +322,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,11 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C20" sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,370 +626,414 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="E21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E21" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E21" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>